<commit_message>
Updated Longitude for Centers
</commit_message>
<xml_diff>
--- a/docs/requirements/Master Data Tables - Test Data/master-registration_center.xlsx
+++ b/docs/requirements/Master Data Tables - Test Data/master-registration_center.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8BFAF1DA-0039-49DD-90DF-6BD964EBD1F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{96D6CF1E-9B32-4899-ACFA-C84A8654A221}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="168">
   <si>
     <t>id</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>بن منصور</t>
-  </si>
-  <si>
-    <t> -6.453275</t>
   </si>
   <si>
     <t>(GTM+01:00) CENTRAL EUROPEAN TIME</t>
@@ -859,7 +856,7 @@
   <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -984,8 +981,8 @@
       <c r="G2">
         <v>34.521169999999998</v>
       </c>
-      <c r="H2" t="s">
-        <v>32</v>
+      <c r="H2">
+        <v>-6.4532749999999997</v>
       </c>
       <c r="I2">
         <v>14022</v>
@@ -994,7 +991,7 @@
         <v>779517433</v>
       </c>
       <c r="K2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L2">
         <v>3</v>
@@ -1018,22 +1015,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" t="s">
         <v>33</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>34</v>
       </c>
-      <c r="U2" t="s">
-        <v>35</v>
-      </c>
       <c r="V2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="13.5" customHeight="1">
@@ -1042,7 +1039,7 @@
         <v>10001</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -1059,8 +1056,8 @@
       <c r="G3">
         <v>34.521169999999998</v>
       </c>
-      <c r="H3" t="s">
-        <v>32</v>
+      <c r="H3">
+        <v>-6.4532749999999997</v>
       </c>
       <c r="I3">
         <v>14022</v>
@@ -1069,7 +1066,7 @@
         <v>944945765</v>
       </c>
       <c r="K3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L3">
         <v>3</v>
@@ -1093,22 +1090,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -1117,7 +1114,7 @@
         <v>10001</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -1134,8 +1131,8 @@
       <c r="G4">
         <v>34.521169999999998</v>
       </c>
-      <c r="H4" t="s">
-        <v>32</v>
+      <c r="H4">
+        <v>-6.4532749999999997</v>
       </c>
       <c r="I4">
         <v>14022</v>
@@ -1144,7 +1141,7 @@
         <v>993556086</v>
       </c>
       <c r="K4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -1168,22 +1165,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -1192,16 +1189,16 @@
         <v>10002</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
         <v>46</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
@@ -1219,7 +1216,7 @@
         <v>753476995</v>
       </c>
       <c r="K5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L5">
         <v>2</v>
@@ -1243,22 +1240,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" t="s">
         <v>33</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>34</v>
       </c>
-      <c r="U5" t="s">
-        <v>35</v>
-      </c>
       <c r="V5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -1267,16 +1264,16 @@
         <v>10002</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>30</v>
@@ -1294,7 +1291,7 @@
         <v>910638389</v>
       </c>
       <c r="K6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -1318,22 +1315,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -1342,16 +1339,16 @@
         <v>10002</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
       <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
         <v>46</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -1369,7 +1366,7 @@
         <v>984996886</v>
       </c>
       <c r="K7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L7">
         <v>2</v>
@@ -1393,22 +1390,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -1417,16 +1414,16 @@
         <v>10003</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
         <v>28</v>
@@ -1444,7 +1441,7 @@
         <v>734239083</v>
       </c>
       <c r="K8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L8">
         <v>4</v>
@@ -1468,22 +1465,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" t="s">
         <v>33</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>34</v>
       </c>
-      <c r="U8" t="s">
-        <v>35</v>
-      </c>
       <c r="V8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1492,16 +1489,16 @@
         <v>10003</v>
       </c>
       <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>30</v>
@@ -1519,7 +1516,7 @@
         <v>910944467</v>
       </c>
       <c r="K9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L9">
         <v>4</v>
@@ -1543,22 +1540,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -1567,16 +1564,16 @@
         <v>10003</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
       <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
         <v>53</v>
-      </c>
-      <c r="E10" t="s">
-        <v>54</v>
       </c>
       <c r="F10" t="s">
         <v>26</v>
@@ -1594,7 +1591,7 @@
         <v>675470523</v>
       </c>
       <c r="K10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L10">
         <v>4</v>
@@ -1618,22 +1615,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -1642,16 +1639,16 @@
         <v>10004</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
         <v>28</v>
@@ -1669,7 +1666,7 @@
         <v>937997757</v>
       </c>
       <c r="K11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L11">
         <v>2</v>
@@ -1693,22 +1690,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S11" t="s">
+        <v>32</v>
+      </c>
+      <c r="T11" t="s">
         <v>33</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>34</v>
       </c>
-      <c r="U11" t="s">
-        <v>35</v>
-      </c>
       <c r="V11" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:24">
@@ -1717,16 +1714,16 @@
         <v>10004</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
         <v>64</v>
-      </c>
-      <c r="E12" t="s">
-        <v>65</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>30</v>
@@ -1744,7 +1741,7 @@
         <v>950807537</v>
       </c>
       <c r="K12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L12">
         <v>2</v>
@@ -1768,22 +1765,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -1792,16 +1789,16 @@
         <v>10004</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
         <v>26</v>
@@ -1819,7 +1816,7 @@
         <v>852492117</v>
       </c>
       <c r="K13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -1843,22 +1840,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1867,16 +1864,16 @@
         <v>10005</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
         <v>26</v>
@@ -1894,7 +1891,7 @@
         <v>887311749</v>
       </c>
       <c r="K14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -1918,22 +1915,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T14" t="s">
         <v>33</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>34</v>
       </c>
-      <c r="U14" t="s">
-        <v>35</v>
-      </c>
       <c r="V14" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1942,16 +1939,16 @@
         <v>10005</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>30</v>
@@ -1969,7 +1966,7 @@
         <v>929072416</v>
       </c>
       <c r="K15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1993,22 +1990,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V15" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -2017,16 +2014,16 @@
         <v>10005</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" t="s">
         <v>26</v>
@@ -2044,7 +2041,7 @@
         <v>658302699</v>
       </c>
       <c r="K16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -2068,22 +2065,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V16" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:24">
@@ -2092,16 +2089,16 @@
         <v>10006</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
@@ -2119,7 +2116,7 @@
         <v>915790305</v>
       </c>
       <c r="K17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L17">
         <v>2</v>
@@ -2143,22 +2140,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S17" t="s">
+        <v>32</v>
+      </c>
+      <c r="T17" t="s">
         <v>33</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>34</v>
       </c>
-      <c r="U17" t="s">
-        <v>35</v>
-      </c>
       <c r="V17" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:24">
@@ -2167,16 +2164,16 @@
         <v>10006</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>30</v>
@@ -2194,7 +2191,7 @@
         <v>722656761</v>
       </c>
       <c r="K18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L18">
         <v>2</v>
@@ -2218,22 +2215,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V18" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:24">
@@ -2242,16 +2239,16 @@
         <v>10006</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
         <v>26</v>
@@ -2269,7 +2266,7 @@
         <v>888439793</v>
       </c>
       <c r="K19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L19">
         <v>2</v>
@@ -2293,22 +2290,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:24">
@@ -2317,16 +2314,16 @@
         <v>10007</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" t="s">
         <v>28</v>
@@ -2344,7 +2341,7 @@
         <v>811552880</v>
       </c>
       <c r="K20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L20">
         <v>2</v>
@@ -2368,22 +2365,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S20" t="s">
+        <v>32</v>
+      </c>
+      <c r="T20" t="s">
         <v>33</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>34</v>
       </c>
-      <c r="U20" t="s">
-        <v>35</v>
-      </c>
       <c r="V20" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:24">
@@ -2392,16 +2389,16 @@
         <v>10007</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>30</v>
@@ -2419,7 +2416,7 @@
         <v>680758944</v>
       </c>
       <c r="K21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L21">
         <v>2</v>
@@ -2443,22 +2440,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V21" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:24">
@@ -2467,16 +2464,16 @@
         <v>10007</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F22" t="s">
         <v>26</v>
@@ -2494,7 +2491,7 @@
         <v>753640112</v>
       </c>
       <c r="K22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L22">
         <v>2</v>
@@ -2518,22 +2515,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V22" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:24">
@@ -2542,16 +2539,16 @@
         <v>10008</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
       </c>
       <c r="D23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" t="s">
         <v>90</v>
-      </c>
-      <c r="E23" t="s">
-        <v>91</v>
       </c>
       <c r="F23" t="s">
         <v>28</v>
@@ -2569,7 +2566,7 @@
         <v>695325692</v>
       </c>
       <c r="K23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -2593,22 +2590,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S23" t="s">
+        <v>32</v>
+      </c>
+      <c r="T23" t="s">
         <v>33</v>
       </c>
-      <c r="T23" t="s">
+      <c r="U23" t="s">
         <v>34</v>
       </c>
-      <c r="U23" t="s">
-        <v>35</v>
-      </c>
       <c r="V23" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:24">
@@ -2617,16 +2614,16 @@
         <v>10008</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>30</v>
@@ -2644,7 +2641,7 @@
         <v>851013196</v>
       </c>
       <c r="K24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L24">
         <v>2</v>
@@ -2668,22 +2665,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V24" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:24">
@@ -2692,16 +2689,16 @@
         <v>10008</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
         <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
         <v>26</v>
@@ -2719,7 +2716,7 @@
         <v>862899075</v>
       </c>
       <c r="K25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L25">
         <v>2</v>
@@ -2743,22 +2740,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V25" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:24">
@@ -2767,16 +2764,16 @@
         <v>10009</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
       <c r="D26" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" t="s">
         <v>98</v>
-      </c>
-      <c r="E26" t="s">
-        <v>99</v>
       </c>
       <c r="F26" t="s">
         <v>28</v>
@@ -2794,7 +2791,7 @@
         <v>745360421</v>
       </c>
       <c r="K26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L26">
         <v>2</v>
@@ -2818,22 +2815,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V26" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:24">
@@ -2842,16 +2839,16 @@
         <v>10009</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>30</v>
@@ -2869,7 +2866,7 @@
         <v>889575995</v>
       </c>
       <c r="K27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L27">
         <v>2</v>
@@ -2893,22 +2890,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V27" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:24">
@@ -2917,16 +2914,16 @@
         <v>10009</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
         <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F28" t="s">
         <v>26</v>
@@ -2944,7 +2941,7 @@
         <v>676186831</v>
       </c>
       <c r="K28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L28">
         <v>2</v>
@@ -2968,22 +2965,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V28" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:24">
@@ -2992,16 +2989,16 @@
         <v>10010</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F29" t="s">
         <v>28</v>
@@ -3019,7 +3016,7 @@
         <v>766074745</v>
       </c>
       <c r="K29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L29">
         <v>2</v>
@@ -3043,22 +3040,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V29" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:24">
@@ -3067,16 +3064,16 @@
         <v>10010</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
         <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>30</v>
@@ -3094,7 +3091,7 @@
         <v>730621636</v>
       </c>
       <c r="K30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L30">
         <v>2</v>
@@ -3118,22 +3115,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V30" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:24">
@@ -3142,16 +3139,16 @@
         <v>10010</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
         <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F31" t="s">
         <v>26</v>
@@ -3169,7 +3166,7 @@
         <v>773606891</v>
       </c>
       <c r="K31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L31">
         <v>2</v>
@@ -3193,22 +3190,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V31" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:24">
@@ -3217,16 +3214,16 @@
         <v>10011</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
         <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F32" t="s">
         <v>28</v>
@@ -3244,7 +3241,7 @@
         <v>787248921</v>
       </c>
       <c r="K32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L32">
         <v>2</v>
@@ -3268,22 +3265,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V32" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:24">
@@ -3292,16 +3289,16 @@
         <v>10011</v>
       </c>
       <c r="B33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C33" t="s">
         <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>30</v>
@@ -3319,7 +3316,7 @@
         <v>966040427</v>
       </c>
       <c r="K33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L33">
         <v>2</v>
@@ -3343,22 +3340,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V33" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:24">
@@ -3367,16 +3364,16 @@
         <v>10011</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F34" t="s">
         <v>26</v>
@@ -3394,7 +3391,7 @@
         <v>878691008</v>
       </c>
       <c r="K34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L34">
         <v>2</v>
@@ -3418,22 +3415,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V34" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:24">
@@ -3442,16 +3439,16 @@
         <v>10012</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
         <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F35" t="s">
         <v>28</v>
@@ -3469,7 +3466,7 @@
         <v>838412388</v>
       </c>
       <c r="K35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L35">
         <v>2</v>
@@ -3493,22 +3490,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V35" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:24">
@@ -3517,16 +3514,16 @@
         <v>10012</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>30</v>
@@ -3544,7 +3541,7 @@
         <v>759605605</v>
       </c>
       <c r="K36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L36">
         <v>2</v>
@@ -3568,22 +3565,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V36" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:24">
@@ -3592,16 +3589,16 @@
         <v>10012</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C37" t="s">
         <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F37" t="s">
         <v>26</v>
@@ -3619,7 +3616,7 @@
         <v>719952201</v>
       </c>
       <c r="K37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L37">
         <v>2</v>
@@ -3643,22 +3640,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V37" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:24">
@@ -3667,16 +3664,16 @@
         <v>10013</v>
       </c>
       <c r="B38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C38" t="s">
         <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F38" t="s">
         <v>28</v>
@@ -3694,7 +3691,7 @@
         <v>751913644</v>
       </c>
       <c r="K38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L38">
         <v>2</v>
@@ -3718,22 +3715,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V38" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:24">
@@ -3742,16 +3739,16 @@
         <v>10013</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C39" t="s">
         <v>25</v>
       </c>
       <c r="D39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>30</v>
@@ -3769,7 +3766,7 @@
         <v>820594414</v>
       </c>
       <c r="K39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L39">
         <v>2</v>
@@ -3793,22 +3790,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V39" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:24">
@@ -3817,16 +3814,16 @@
         <v>10013</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C40" t="s">
         <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F40" t="s">
         <v>26</v>
@@ -3844,7 +3841,7 @@
         <v>956537434</v>
       </c>
       <c r="K40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L40">
         <v>2</v>
@@ -3868,22 +3865,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V40" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:24">
@@ -3892,16 +3889,16 @@
         <v>10014</v>
       </c>
       <c r="B41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C41" t="s">
         <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F41" t="s">
         <v>28</v>
@@ -3919,7 +3916,7 @@
         <v>965639376</v>
       </c>
       <c r="K41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L41">
         <v>2</v>
@@ -3943,22 +3940,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V41" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:24">
@@ -3967,16 +3964,16 @@
         <v>10014</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>30</v>
@@ -3994,7 +3991,7 @@
         <v>885430659</v>
       </c>
       <c r="K42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L42">
         <v>2</v>
@@ -4018,22 +4015,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V42" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:24">
@@ -4042,16 +4039,16 @@
         <v>10014</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C43" t="s">
         <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F43" t="s">
         <v>26</v>
@@ -4069,7 +4066,7 @@
         <v>781039430</v>
       </c>
       <c r="K43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L43">
         <v>2</v>
@@ -4093,22 +4090,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V43" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:24">
@@ -4117,16 +4114,16 @@
         <v>10015</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
       </c>
       <c r="D44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F44" t="s">
         <v>28</v>
@@ -4144,7 +4141,7 @@
         <v>803062069</v>
       </c>
       <c r="K44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L44">
         <v>2</v>
@@ -4168,22 +4165,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V44" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:24">
@@ -4192,16 +4189,16 @@
         <v>10015</v>
       </c>
       <c r="B45" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" t="s">
         <v>134</v>
       </c>
-      <c r="C45" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45" t="s">
-        <v>135</v>
-      </c>
       <c r="E45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>30</v>
@@ -4219,7 +4216,7 @@
         <v>802491003</v>
       </c>
       <c r="K45" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L45">
         <v>2</v>
@@ -4243,22 +4240,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V45" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:24">
@@ -4267,16 +4264,16 @@
         <v>10015</v>
       </c>
       <c r="B46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C46" t="s">
         <v>25</v>
       </c>
       <c r="D46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F46" t="s">
         <v>26</v>
@@ -4294,7 +4291,7 @@
         <v>731435978</v>
       </c>
       <c r="K46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L46">
         <v>2</v>
@@ -4318,22 +4315,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="S46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V46" s="2" t="b">
         <v>1</v>
       </c>
       <c r="W46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>